<commit_message>
2023-10-30 17:23:35 Update Excel file
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>規劃時間</t>
   </si>
@@ -34,22 +34,16 @@
     <t>109120595628011,127520840434805,17841439965935599,</t>
   </si>
   <si>
-    <t>/Users/jishuliu/Desktop/hkshop/data/20231030_superdelivery/【日本直送】 HEIKO(ヘイコー)  ヘイコー 注意喚起シール カッター注意 48枚  Heiko 警告貼紙切割器警告 48 張  一色入</t>
+    <t>/Users/jishuliu/Desktop/hkshop/data/20231030_superdelivery/【日本直送】 ササガワ　ＩＴ事業部（すべてのジャンル）  荷札シール　取扱注意  行李標籤貼紙 小心輕放  一色入</t>
   </si>
   <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_97673231495526381841.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_24630472784114198014.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_52511978479840678704.jpg</t>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_40870190220846178232.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_22676963380593410709.jpg</t>
   </si>
   <si>
-    <t>/Users/jishuliu/Desktop/hkshop/data/20231030_superdelivery/【日本直送】 HEIKO(ヘイコー)  おにぎりシール　梅　98片  飯糰貼紙梅花 98枚  一色入</t>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_03156904136975129854.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_65403258431629315721.jpg</t>
   </si>
   <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_72387604435217684814.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_51848917452407100069.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_82770163907626825089.jpg</t>
-  </si>
-  <si>
-    <t>/Users/jishuliu/Desktop/hkshop/data/20231030_superdelivery/【日本直送】 HEIKO(ヘイコー)  おにぎりシール　鮭　98片  飯糰貼紙98片鮭魚  一色入</t>
-  </si>
-  <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_35185681854805650421.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_08046008794665298458.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_27328565906727858090.jpg</t>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_46386897831229038267.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_35055401077700880486.jpg</t>
   </si>
   <si>
     <t/>
@@ -65,7 +59,14 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,148 +522,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1018,15 +1019,15 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="23.3846153846154" customWidth="1"/>
+    <col min="1" max="1" width="27.3942307692308" customWidth="1"/>
     <col min="2" max="2" width="100.5" customWidth="1"/>
-    <col min="3" max="3" width="193.5" customWidth="1"/>
-    <col min="4" max="4" width="367.5" customWidth="1"/>
+    <col min="3" max="3" width="174" customWidth="1"/>
+    <col min="4" max="4" width="244.5" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1049,7 +1050,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>45229.6875</v>
+        <v>45229.7291666667</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1063,33 +1064,33 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>45229.7083333333</v>
+        <v>45229.7708333333</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>45229.7291666667</v>
+        <v>45229.75</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023-10-31 14:51:43 Update Excel file
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15040"/>
+    <workbookView windowHeight="15020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>規劃時間</t>
   </si>
@@ -31,19 +31,19 @@
     <t>內容</t>
   </si>
   <si>
-    <t>109120595628011,127520840434805,17841439965935599,</t>
+    <t>127520840434805,103482326003878,17841461742288388,17841456036806884</t>
   </si>
   <si>
-    <t>/Users/jishuliu/Desktop/hkshop/data/20231030_superdelivery/【日本直送】 ササガワ　ＩＴ事業部（すべてのジャンル）  荷札シール　取扱注意  行李標籤貼紙 小心輕放  一色入</t>
+    <t>/Users/jishuliu/Desktop/hkshop/data/20231031_superdelivery/【日本直送】 ササガワ　ＩＴ事業部（すべてのジャンル）  荷札シール　取扱注意  行李標籤貼紙 小心輕放  一色入</t>
   </si>
   <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_40870190220846178232.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_22676963380593410709.jpg</t>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_84835830603419215654.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_46914841642146126210.jpg</t>
   </si>
   <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_03156904136975129854.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_65403258431629315721.jpg</t>
+    <t>/Users/jishuliu/Desktop/hkshop/data/20231031_superdelivery/【日本直送】 HEIKO(ヘイコー)  ヘイコー 注意喚起シール カッター注意 48枚  Heiko 警告貼紙切割器警告 48 張  一色入</t>
   </si>
   <si>
-    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_46386897831229038267.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_35055401077700880486.jpg</t>
+    <t>https://shopage.s3.amazonaws.com/media/f854/615273998674_32746879691743666134.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_78459562396381333295.jpg,https://shopage.s3.amazonaws.com/media/f854/615273998674_04964299814229126722.jpg</t>
   </si>
   <si>
     <t/>
@@ -59,14 +59,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,154 +515,155 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1016,18 +1010,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="27.3942307692308" customWidth="1"/>
+    <col min="1" max="1" width="36.2115384615385" customWidth="1"/>
     <col min="2" max="2" width="100.5" customWidth="1"/>
-    <col min="3" max="3" width="174" customWidth="1"/>
-    <col min="4" max="4" width="244.5" customWidth="1"/>
+    <col min="3" max="3" width="193.5" customWidth="1"/>
+    <col min="4" max="4" width="367.5" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1050,9 +1044,9 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>45229.7291666667</v>
-      </c>
-      <c r="B2" t="s">
+        <v>45230.625</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -1062,34 +1056,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>45229.7708333333</v>
-      </c>
-      <c r="B3" t="s">
+        <v>45230.6458333333</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>45229.75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>